<commit_message>
We support double border and thus have to update a cell and its left/top/right/bottom neighbor cells. Thus have to change test case to move from A2 to A3.
</commit_message>
<xml_diff>
--- a/zss.test/src/main/webapp/issue3/book/760-refresh.xlsx
+++ b/zss.test/src/main/webapp/issue3/book/760-refresh.xlsx
@@ -342,16 +342,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2"/>
+  <dimension ref="A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="2" spans="1:1">
-      <c r="A2">
+    <row r="3" spans="1:1">
+      <c r="A3">
         <f>A1+1</f>
         <v>1</v>
       </c>

</xml_diff>